<commit_message>
Implementado cadastro de usuário + área de cadastro
</commit_message>
<xml_diff>
--- a/Backlog_Sprint_2.xlsx
+++ b/Backlog_Sprint_2.xlsx
@@ -158,7 +158,7 @@
             <text:p>4</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Cadastro funcional com registro no banco de dados</text:p>
+            <text:p>Cadastro aplicar usuário no banco</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
@@ -185,9 +185,9 @@
 <file path=meta.xml><?xml version="1.0" encoding="utf-8"?>
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" office:version="1.3">
   <office:meta>
-    <dc:date>2021-11-23T14:32:05.900000000</dc:date>
-    <meta:editing-duration>PT13M12S</meta:editing-duration>
-    <meta:editing-cycles>5</meta:editing-cycles>
+    <dc:date>2021-11-23T14:56:22.552000000</dc:date>
+    <meta:editing-duration>PT37M28S</meta:editing-duration>
+    <meta:editing-cycles>6</meta:editing-cycles>
     <meta:generator>LibreOffice/7.1.0.3$Windows_X86_64 LibreOffice_project/f6099ecf3d29644b5008cc8f48f42f4a40986e4c</meta:generator>
     <meta:document-statistic meta:table-count="1" meta:cell-count="18" meta:object-count="0"/>
   </office:meta>
@@ -208,7 +208,7 @@
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Planilha1">
               <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">12</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">8</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>

</xml_diff>